<commit_message>
working on YUN flow
</commit_message>
<xml_diff>
--- a/docs/arduino mailbox flow.xlsx
+++ b/docs/arduino mailbox flow.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
   <si>
     <t xml:space="preserve">Mailbox Sensor Logic (Arduino)</t>
   </si>
@@ -28,6 +28,111 @@
     <t xml:space="preserve">Normal Operation Action</t>
   </si>
   <si>
+    <t xml:space="preserve">Red (mailbox radio) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green (house radio)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yellow (house text)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">initialize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lights off &amp; wait for mailbox open (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lights off &amp; wait for RX Red (4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mailbox open</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red led on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tell gate we ‘got mail’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TX Red continuously</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gate received ‘got mail’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX Red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tell mailbox + house we ‘got mail’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TX Green continuously</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mailbox received ‘got mail’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX Green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stop TX (step 3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">green led on for 20 seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reset mailbox to ‘waiting for mail’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red led off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">house received ‘got mail’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dig pin HIGH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">green led on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tell Bob &amp; Susan they ‘got mail’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beep every 8 seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">House tell gate we ‘got mail’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TX Yellow for 10 seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX Yellow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stop TX (step 6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yellow led on for 10 seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">press reset button at house</t>
+  </si>
+  <si>
+    <t xml:space="preserve">green led off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stop beeping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">go to step 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Action</t>
+  </si>
+  <si>
     <t xml:space="preserve">Red (mailbox) </t>
   </si>
   <si>
@@ -35,105 +140,6 @@
   </si>
   <si>
     <t xml:space="preserve">Yellow (House)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">initialize</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lights off &amp; wait for mailbox open (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lights off &amp; wait for RX Red (4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lights off &amp; wait for RX Green (12)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mailbox open</t>
-  </si>
-  <si>
-    <t xml:space="preserve">red led on</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tell gate we ‘got mail’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TX Red continuously</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gate received ‘got mail’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RX Red</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tell mailbox + house we ‘got mail’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TX Green continuously</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mailbox received ‘got mail’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RX Green</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stop TX (step 3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">green led on for 20 seconds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reset mailbox to ‘waiting for mail’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">red led off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">house received ‘got mail’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">green led on</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tell Bob &amp; Susan they ‘got mail’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beep every 8 seconds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">House tell gate we ‘got mail’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TX Yellow for 10 seconds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RX Yellow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stop TX (step 6)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yellow led on for 10 seconds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">press reset button at house</t>
-  </si>
-  <si>
-    <t xml:space="preserve">green led off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stop beeping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">go to step 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Action</t>
   </si>
   <si>
     <t xml:space="preserve">connect Test jumpers to +3.7 volts on each radio board</t>
@@ -477,7 +483,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -514,7 +520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
         <v>1</v>
       </c>
@@ -527,19 +533,17 @@
       <c r="D3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>8</v>
-      </c>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>10</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -549,10 +553,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>12</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -562,11 +566,11 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -577,34 +581,32 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="11"/>
@@ -615,7 +617,7 @@
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="11"/>
@@ -626,7 +628,7 @@
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="11"/>
@@ -636,10 +638,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="11"/>
@@ -649,12 +651,14 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="E13" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -665,7 +669,7 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -673,12 +677,12 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -686,12 +690,12 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="11"/>
       <c r="E16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -699,11 +703,11 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" s="3"/>
     </row>
@@ -714,7 +718,7 @@
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E18" s="3"/>
     </row>
@@ -725,7 +729,7 @@
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E19" s="3"/>
     </row>
@@ -736,7 +740,7 @@
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E20" s="3"/>
     </row>
@@ -745,12 +749,12 @@
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -761,7 +765,7 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -769,7 +773,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -784,16 +788,16 @@
     </row>
     <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>2</v>
-      </c>
       <c r="D25" s="6" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -801,16 +805,16 @@
         <v>22</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -818,11 +822,11 @@
         <v>23</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="19" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E27" s="19"/>
     </row>
@@ -831,14 +835,14 @@
         <v>24</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D28" s="19"/>
       <c r="E28" s="19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -846,14 +850,14 @@
         <v>25</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D29" s="19"/>
       <c r="E29" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -861,14 +865,14 @@
         <v>26</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D30" s="19"/>
       <c r="E30" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -876,11 +880,11 @@
         <v>27</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E31" s="19"/>
     </row>
@@ -889,11 +893,11 @@
         <v>28</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C32" s="19"/>
       <c r="D32" s="19" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E32" s="19"/>
     </row>
@@ -902,11 +906,11 @@
         <v>29</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E33" s="19"/>
     </row>
@@ -915,17 +919,17 @@
         <v>30</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C34" s="19"/>
       <c r="D34" s="19" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E34" s="19"/>
     </row>
     <row r="35" customFormat="false" ht="47.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="20" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D35" s="0"/>
     </row>

</xml_diff>